<commit_message>
Ash test chamber concepts (2nd BOM redundant)
</commit_message>
<xml_diff>
--- a/Volcanic_Ash_FYP_BOM_1.xlsx
+++ b/Volcanic_Ash_FYP_BOM_1.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>Order 1</t>
   </si>
@@ -87,6 +87,12 @@
   </si>
   <si>
     <t>Shinyei PPD42NS Optical Dust Sensor</t>
+  </si>
+  <si>
+    <t>Order Lodged with</t>
+  </si>
+  <si>
+    <t>UC ECE Dept.</t>
   </si>
 </sst>
 </file>
@@ -414,16 +420,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:K15"/>
+  <dimension ref="B3:K17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="35.59765625" customWidth="1"/>
-    <col min="3" max="3" width="11.09765625" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
     <col min="4" max="4" width="17.09765625" customWidth="1"/>
     <col min="5" max="5" width="23.5" customWidth="1"/>
     <col min="6" max="6" width="13.69921875" customWidth="1"/>
@@ -440,107 +446,70 @@
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
+      <c r="B4" s="1"/>
+      <c r="K4" s="1"/>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K5" s="1"/>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C6" s="2">
         <v>42488</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="C5" s="2"/>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C7" s="2"/>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
         <v>13</v>
       </c>
-      <c r="C6">
+      <c r="C8">
         <v>1.44</v>
       </c>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B8" s="1" t="s">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B10" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="H10" s="1" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9">
-        <v>6.8</v>
-      </c>
-      <c r="D9">
-        <f>$C9*$C$6</f>
-        <v>9.7919999999999998</v>
-      </c>
-      <c r="E9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <f>$F9*$C$6</f>
-        <v>0</v>
-      </c>
-      <c r="H9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10">
-        <v>33</v>
-      </c>
-      <c r="D10">
-        <f>$C10*$C$6</f>
-        <v>47.519999999999996</v>
-      </c>
-      <c r="E10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <f>$F10*$C$6</f>
-        <v>0</v>
-      </c>
-      <c r="H10" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C11">
-        <v>25.5</v>
+        <v>6.8</v>
       </c>
       <c r="D11">
-        <f>$C11*$C$6</f>
-        <v>36.72</v>
+        <f>$C11*$C$8</f>
+        <v>9.7919999999999998</v>
       </c>
       <c r="E11" t="s">
         <v>9</v>
@@ -549,23 +518,23 @@
         <v>0</v>
       </c>
       <c r="G11">
-        <f>$F11*$C$6</f>
+        <f>$F11*$C$8</f>
         <v>0</v>
       </c>
       <c r="H11" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="C12">
-        <v>10.5</v>
+        <v>33</v>
       </c>
       <c r="D12">
-        <f>$C12*$C$6</f>
-        <v>15.12</v>
+        <f>$C12*$C$8</f>
+        <v>47.519999999999996</v>
       </c>
       <c r="E12" t="s">
         <v>9</v>
@@ -574,19 +543,69 @@
         <v>0</v>
       </c>
       <c r="G12">
-        <f>$F12*$C$6</f>
+        <f>$F12*$C$8</f>
         <v>0</v>
       </c>
       <c r="H12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13">
+        <v>25.5</v>
+      </c>
+      <c r="D13">
+        <f>$C13*$C$8</f>
+        <v>36.72</v>
+      </c>
+      <c r="E13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <f>$F13*$C$8</f>
+        <v>0</v>
+      </c>
+      <c r="H13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14">
+        <v>10.5</v>
+      </c>
+      <c r="D14">
+        <f>$C14*$C$8</f>
+        <v>15.12</v>
+      </c>
+      <c r="E14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <f>$F14*$C$8</f>
+        <v>0</v>
+      </c>
+      <c r="H14" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B15" s="1" t="s">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B17" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C15">
-        <f>SUM(D9:D11,G9:G11)</f>
+      <c r="C17">
+        <f>SUM(D11:D13,G11:G13)</f>
         <v>94.031999999999996</v>
       </c>
     </row>

</xml_diff>